<commit_message>
add more dummy data for testing
</commit_message>
<xml_diff>
--- a/dataset/dummy.xlsx
+++ b/dataset/dummy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liche\Desktop\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EBD715-5A37-4CCB-A185-79E2BBE08522}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00DFBEF-0728-4C8C-8A54-E2DAC643ED5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="20460" windowHeight="10920" xr2:uid="{488C3E08-5F7E-46E2-9E12-5158F07ED5AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{488C3E08-5F7E-46E2-9E12-5158F07ED5AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -400,19 +408,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E46C1A07-1C02-4A63-A93F-45EA90516973}">
-  <dimension ref="A1:H68"/>
+  <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="I214" sqref="I214"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,7 +446,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>238196066</v>
       </c>
@@ -464,7 +472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>238295782</v>
       </c>
@@ -491,7 +499,7 @@
         <v>9.9715999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>238396007</v>
       </c>
@@ -518,7 +526,7 @@
         <v>0.10022499999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>238496266</v>
       </c>
@@ -545,7 +553,7 @@
         <v>0.100259</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>238595905</v>
       </c>
@@ -572,7 +580,7 @@
         <v>9.9639000000000005E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>238695724</v>
       </c>
@@ -599,7 +607,7 @@
         <v>9.9819000000000005E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>238795906</v>
       </c>
@@ -626,7 +634,7 @@
         <v>0.10018199999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>238895789</v>
       </c>
@@ -653,7 +661,7 @@
         <v>9.9883E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>238995782</v>
       </c>
@@ -680,7 +688,7 @@
         <v>9.9992999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>239096109</v>
       </c>
@@ -707,7 +715,7 @@
         <v>0.100327</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>239195811</v>
       </c>
@@ -734,7 +742,7 @@
         <v>9.9701999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>239296010</v>
       </c>
@@ -761,7 +769,7 @@
         <v>0.100199</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>239395862</v>
       </c>
@@ -788,7 +796,7 @@
         <v>9.9851999999999996E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>239495888</v>
       </c>
@@ -815,7 +823,7 @@
         <v>0.100026</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>239595759</v>
       </c>
@@ -842,7 +850,7 @@
         <v>9.9871000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>239696195</v>
       </c>
@@ -869,7 +877,7 @@
         <v>0.100436</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>239796002</v>
       </c>
@@ -896,7 +904,7 @@
         <v>9.9807000000000007E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>239895871</v>
       </c>
@@ -923,7 +931,7 @@
         <v>9.9868999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>239996303</v>
       </c>
@@ -950,7 +958,7 @@
         <v>0.10043199999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>240096233</v>
       </c>
@@ -977,7 +985,7 @@
         <v>9.9930000000000005E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>240196119</v>
       </c>
@@ -1004,7 +1012,7 @@
         <v>9.9886000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>240296330</v>
       </c>
@@ -1031,7 +1039,7 @@
         <v>0.10021099999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>240396213</v>
       </c>
@@ -1058,7 +1066,7 @@
         <v>9.9883E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>240496036</v>
       </c>
@@ -1085,7 +1093,7 @@
         <v>9.9822999999999995E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>240596269</v>
       </c>
@@ -1112,7 +1120,7 @@
         <v>0.100233</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>240696119</v>
       </c>
@@ -1139,7 +1147,7 @@
         <v>9.9849999999999994E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>240796097</v>
       </c>
@@ -1166,7 +1174,7 @@
         <v>9.9977999999999997E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>240896330</v>
       </c>
@@ -1193,7 +1201,7 @@
         <v>0.100233</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>240996055</v>
       </c>
@@ -1220,7 +1228,7 @@
         <v>9.9724999999999994E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>241096077</v>
       </c>
@@ -1247,7 +1255,7 @@
         <v>0.100022</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>241196132</v>
       </c>
@@ -1274,7 +1282,7 @@
         <v>0.10005500000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>241296253</v>
       </c>
@@ -1301,7 +1309,7 @@
         <v>0.100121</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>241396206</v>
       </c>
@@ -1328,7 +1336,7 @@
         <v>9.9953E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>241496354</v>
       </c>
@@ -1355,7 +1363,7 @@
         <v>0.100148</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>241596228</v>
       </c>
@@ -1382,7 +1390,7 @@
         <v>9.9874000000000004E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>241696235</v>
       </c>
@@ -1409,7 +1417,7 @@
         <v>0.100007</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>241796313</v>
       </c>
@@ -1436,7 +1444,7 @@
         <v>0.100078</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>241896093</v>
       </c>
@@ -1463,7 +1471,7 @@
         <v>9.9779999999999994E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>241996383</v>
       </c>
@@ -1490,7 +1498,7 @@
         <v>0.10029</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>242096359</v>
       </c>
@@ -1517,7 +1525,7 @@
         <v>9.9975999999999995E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>242196269</v>
       </c>
@@ -1544,7 +1552,7 @@
         <v>9.9909999999999999E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>242296066</v>
       </c>
@@ -1571,7 +1579,7 @@
         <v>9.9796999999999997E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>242396272</v>
       </c>
@@ -1598,7 +1606,7 @@
         <v>0.100206</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>242496465</v>
       </c>
@@ -1625,7 +1633,7 @@
         <v>0.100193</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>242596418</v>
       </c>
@@ -1652,7 +1660,7 @@
         <v>9.9953E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>242696487</v>
       </c>
@@ -1679,7 +1687,7 @@
         <v>0.10006900000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>242796403</v>
       </c>
@@ -1706,7 +1714,7 @@
         <v>9.9916000000000005E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>242896391</v>
       </c>
@@ -1733,7 +1741,7 @@
         <v>9.9987999999999994E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>242996480</v>
       </c>
@@ -1760,7 +1768,7 @@
         <v>0.100089</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>243096547</v>
       </c>
@@ -1787,7 +1795,7 @@
         <v>0.100067</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>243196455</v>
       </c>
@@ -1814,7 +1822,7 @@
         <v>9.9907999999999997E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>243296570</v>
       </c>
@@ -1841,7 +1849,7 @@
         <v>0.100115</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>243396399</v>
       </c>
@@ -1868,7 +1876,7 @@
         <v>9.9829000000000001E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>243496412</v>
       </c>
@@ -1895,7 +1903,7 @@
         <v>0.100013</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>243596450</v>
       </c>
@@ -1922,7 +1930,7 @@
         <v>0.100038</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>243697005</v>
       </c>
@@ -1949,7 +1957,7 @@
         <v>0.10055500000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>243795918</v>
       </c>
@@ -1976,7 +1984,7 @@
         <v>9.8913000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>243896363</v>
       </c>
@@ -2003,7 +2011,7 @@
         <v>0.10044500000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>243996346</v>
       </c>
@@ -2030,7 +2038,7 @@
         <v>9.9983000000000002E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>244096384</v>
       </c>
@@ -2057,7 +2065,7 @@
         <v>0.100038</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>244196445</v>
       </c>
@@ -2084,7 +2092,7 @@
         <v>0.100061</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>244296074</v>
       </c>
@@ -2111,7 +2119,7 @@
         <v>9.9628999999999995E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>244396065</v>
       </c>
@@ -2138,7 +2146,7 @@
         <v>9.9990999999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>244496275</v>
       </c>
@@ -2165,7 +2173,7 @@
         <v>0.10020999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>244596100</v>
       </c>
@@ -2192,7 +2200,7 @@
         <v>9.9824999999999997E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>244696091</v>
       </c>
@@ -2219,7 +2227,7 @@
         <v>9.9990999999999997E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>244796240</v>
       </c>
@@ -2244,6 +2252,2646 @@
       <c r="H68">
         <f t="shared" ref="H68" si="1">(A68-A67)/1000000</f>
         <v>0.100149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>1500</v>
+      </c>
+      <c r="C69">
+        <v>1500</v>
+      </c>
+      <c r="D69">
+        <v>1500</v>
+      </c>
+      <c r="E69">
+        <v>1500</v>
+      </c>
+      <c r="F69">
+        <v>1500</v>
+      </c>
+      <c r="G69">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>1500</v>
+      </c>
+      <c r="C70">
+        <v>1500</v>
+      </c>
+      <c r="D70">
+        <v>1500</v>
+      </c>
+      <c r="E70">
+        <v>1500</v>
+      </c>
+      <c r="F70">
+        <v>1500</v>
+      </c>
+      <c r="G70">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>1500</v>
+      </c>
+      <c r="C71">
+        <v>1500</v>
+      </c>
+      <c r="D71">
+        <v>1500</v>
+      </c>
+      <c r="E71">
+        <v>1500</v>
+      </c>
+      <c r="F71">
+        <v>1500</v>
+      </c>
+      <c r="G71">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>1500</v>
+      </c>
+      <c r="C72">
+        <v>1500</v>
+      </c>
+      <c r="D72">
+        <v>1500</v>
+      </c>
+      <c r="E72">
+        <v>1500</v>
+      </c>
+      <c r="F72">
+        <v>1500</v>
+      </c>
+      <c r="G72">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>1500</v>
+      </c>
+      <c r="C73">
+        <v>1500</v>
+      </c>
+      <c r="D73">
+        <v>1500</v>
+      </c>
+      <c r="E73">
+        <v>1500</v>
+      </c>
+      <c r="F73">
+        <v>1500</v>
+      </c>
+      <c r="G73">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>1500</v>
+      </c>
+      <c r="C74">
+        <v>1500</v>
+      </c>
+      <c r="D74">
+        <v>1500</v>
+      </c>
+      <c r="E74">
+        <v>1500</v>
+      </c>
+      <c r="F74">
+        <v>1500</v>
+      </c>
+      <c r="G74">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>1500</v>
+      </c>
+      <c r="C75">
+        <v>1500</v>
+      </c>
+      <c r="D75">
+        <v>1500</v>
+      </c>
+      <c r="E75">
+        <v>1500</v>
+      </c>
+      <c r="F75">
+        <v>1500</v>
+      </c>
+      <c r="G75">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>1500</v>
+      </c>
+      <c r="C76">
+        <v>1500</v>
+      </c>
+      <c r="D76">
+        <v>1500</v>
+      </c>
+      <c r="E76">
+        <v>1500</v>
+      </c>
+      <c r="F76">
+        <v>1500</v>
+      </c>
+      <c r="G76">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>1500</v>
+      </c>
+      <c r="C77">
+        <v>1500</v>
+      </c>
+      <c r="D77">
+        <v>1500</v>
+      </c>
+      <c r="E77">
+        <v>1500</v>
+      </c>
+      <c r="F77">
+        <v>1500</v>
+      </c>
+      <c r="G77">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>1500</v>
+      </c>
+      <c r="C78">
+        <v>1500</v>
+      </c>
+      <c r="D78">
+        <v>1500</v>
+      </c>
+      <c r="E78">
+        <v>1500</v>
+      </c>
+      <c r="F78">
+        <v>1500</v>
+      </c>
+      <c r="G78">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>1500</v>
+      </c>
+      <c r="C79">
+        <v>1500</v>
+      </c>
+      <c r="D79">
+        <v>1500</v>
+      </c>
+      <c r="E79">
+        <v>1500</v>
+      </c>
+      <c r="F79">
+        <v>1500</v>
+      </c>
+      <c r="G79">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>1500</v>
+      </c>
+      <c r="C80">
+        <v>1500</v>
+      </c>
+      <c r="D80">
+        <v>1500</v>
+      </c>
+      <c r="E80">
+        <v>1500</v>
+      </c>
+      <c r="F80">
+        <v>1500</v>
+      </c>
+      <c r="G80">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>1500</v>
+      </c>
+      <c r="C81">
+        <v>1500</v>
+      </c>
+      <c r="D81">
+        <v>1500</v>
+      </c>
+      <c r="E81">
+        <v>1500</v>
+      </c>
+      <c r="F81">
+        <v>1500</v>
+      </c>
+      <c r="G81">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>1500</v>
+      </c>
+      <c r="C82">
+        <v>1500</v>
+      </c>
+      <c r="D82">
+        <v>1500</v>
+      </c>
+      <c r="E82">
+        <v>1500</v>
+      </c>
+      <c r="F82">
+        <v>1500</v>
+      </c>
+      <c r="G82">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>1500</v>
+      </c>
+      <c r="C83">
+        <v>1500</v>
+      </c>
+      <c r="D83">
+        <v>1500</v>
+      </c>
+      <c r="E83">
+        <v>1500</v>
+      </c>
+      <c r="F83">
+        <v>1500</v>
+      </c>
+      <c r="G83">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>1500</v>
+      </c>
+      <c r="C84">
+        <v>1500</v>
+      </c>
+      <c r="D84">
+        <v>1500</v>
+      </c>
+      <c r="E84">
+        <v>1500</v>
+      </c>
+      <c r="F84">
+        <v>1500</v>
+      </c>
+      <c r="G84">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>1500</v>
+      </c>
+      <c r="C85">
+        <v>1500</v>
+      </c>
+      <c r="D85">
+        <v>1500</v>
+      </c>
+      <c r="E85">
+        <v>1500</v>
+      </c>
+      <c r="F85">
+        <v>1500</v>
+      </c>
+      <c r="G85">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>1500</v>
+      </c>
+      <c r="C86">
+        <v>1500</v>
+      </c>
+      <c r="D86">
+        <v>1500</v>
+      </c>
+      <c r="E86">
+        <v>1500</v>
+      </c>
+      <c r="F86">
+        <v>1500</v>
+      </c>
+      <c r="G86">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>1500</v>
+      </c>
+      <c r="C87">
+        <v>1500</v>
+      </c>
+      <c r="D87">
+        <v>1500</v>
+      </c>
+      <c r="E87">
+        <v>1500</v>
+      </c>
+      <c r="F87">
+        <v>1500</v>
+      </c>
+      <c r="G87">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>1500</v>
+      </c>
+      <c r="C88">
+        <v>1500</v>
+      </c>
+      <c r="D88">
+        <v>1500</v>
+      </c>
+      <c r="E88">
+        <v>1500</v>
+      </c>
+      <c r="F88">
+        <v>1500</v>
+      </c>
+      <c r="G88">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>1500</v>
+      </c>
+      <c r="C89">
+        <v>1500</v>
+      </c>
+      <c r="D89">
+        <v>1500</v>
+      </c>
+      <c r="E89">
+        <v>1500</v>
+      </c>
+      <c r="F89">
+        <v>1500</v>
+      </c>
+      <c r="G89">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>1500</v>
+      </c>
+      <c r="C90">
+        <v>1500</v>
+      </c>
+      <c r="D90">
+        <v>1500</v>
+      </c>
+      <c r="E90">
+        <v>1500</v>
+      </c>
+      <c r="F90">
+        <v>1500</v>
+      </c>
+      <c r="G90">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>1500</v>
+      </c>
+      <c r="C91">
+        <v>1500</v>
+      </c>
+      <c r="D91">
+        <v>1500</v>
+      </c>
+      <c r="E91">
+        <v>1500</v>
+      </c>
+      <c r="F91">
+        <v>1500</v>
+      </c>
+      <c r="G91">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>1500</v>
+      </c>
+      <c r="C92">
+        <v>1500</v>
+      </c>
+      <c r="D92">
+        <v>1500</v>
+      </c>
+      <c r="E92">
+        <v>1500</v>
+      </c>
+      <c r="F92">
+        <v>1500</v>
+      </c>
+      <c r="G92">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>1500</v>
+      </c>
+      <c r="C93">
+        <v>1500</v>
+      </c>
+      <c r="D93">
+        <v>1500</v>
+      </c>
+      <c r="E93">
+        <v>1500</v>
+      </c>
+      <c r="F93">
+        <v>1500</v>
+      </c>
+      <c r="G93">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>1500</v>
+      </c>
+      <c r="C94">
+        <v>1500</v>
+      </c>
+      <c r="D94">
+        <v>1500</v>
+      </c>
+      <c r="E94">
+        <v>1500</v>
+      </c>
+      <c r="F94">
+        <v>1500</v>
+      </c>
+      <c r="G94">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>1500</v>
+      </c>
+      <c r="C95">
+        <v>1500</v>
+      </c>
+      <c r="D95">
+        <v>1500</v>
+      </c>
+      <c r="E95">
+        <v>1500</v>
+      </c>
+      <c r="F95">
+        <v>1500</v>
+      </c>
+      <c r="G95">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>1500</v>
+      </c>
+      <c r="C96">
+        <v>1500</v>
+      </c>
+      <c r="D96">
+        <v>1500</v>
+      </c>
+      <c r="E96">
+        <v>1500</v>
+      </c>
+      <c r="F96">
+        <v>1500</v>
+      </c>
+      <c r="G96">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>1500</v>
+      </c>
+      <c r="C97">
+        <v>1500</v>
+      </c>
+      <c r="D97">
+        <v>1500</v>
+      </c>
+      <c r="E97">
+        <v>1500</v>
+      </c>
+      <c r="F97">
+        <v>1500</v>
+      </c>
+      <c r="G97">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>1500</v>
+      </c>
+      <c r="C98">
+        <v>1500</v>
+      </c>
+      <c r="D98">
+        <v>1500</v>
+      </c>
+      <c r="E98">
+        <v>1500</v>
+      </c>
+      <c r="F98">
+        <v>1500</v>
+      </c>
+      <c r="G98">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>1500</v>
+      </c>
+      <c r="C99">
+        <v>1500</v>
+      </c>
+      <c r="D99">
+        <v>1500</v>
+      </c>
+      <c r="E99">
+        <v>1500</v>
+      </c>
+      <c r="F99">
+        <v>1500</v>
+      </c>
+      <c r="G99">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <v>1500</v>
+      </c>
+      <c r="C100">
+        <v>1500</v>
+      </c>
+      <c r="D100">
+        <v>1500</v>
+      </c>
+      <c r="E100">
+        <v>1500</v>
+      </c>
+      <c r="F100">
+        <v>1500</v>
+      </c>
+      <c r="G100">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B101">
+        <v>1500</v>
+      </c>
+      <c r="C101">
+        <v>1500</v>
+      </c>
+      <c r="D101">
+        <v>1500</v>
+      </c>
+      <c r="E101">
+        <v>1500</v>
+      </c>
+      <c r="F101">
+        <v>1500</v>
+      </c>
+      <c r="G101">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>1500</v>
+      </c>
+      <c r="C102">
+        <v>1500</v>
+      </c>
+      <c r="D102">
+        <v>1500</v>
+      </c>
+      <c r="E102">
+        <v>1500</v>
+      </c>
+      <c r="F102">
+        <v>1500</v>
+      </c>
+      <c r="G102">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>1500</v>
+      </c>
+      <c r="C103">
+        <v>1500</v>
+      </c>
+      <c r="D103">
+        <v>1500</v>
+      </c>
+      <c r="E103">
+        <v>1500</v>
+      </c>
+      <c r="F103">
+        <v>1500</v>
+      </c>
+      <c r="G103">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>1500</v>
+      </c>
+      <c r="C104">
+        <v>1500</v>
+      </c>
+      <c r="D104">
+        <v>1500</v>
+      </c>
+      <c r="E104">
+        <v>1500</v>
+      </c>
+      <c r="F104">
+        <v>1500</v>
+      </c>
+      <c r="G104">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>1500</v>
+      </c>
+      <c r="C105">
+        <v>1500</v>
+      </c>
+      <c r="D105">
+        <v>1500</v>
+      </c>
+      <c r="E105">
+        <v>1500</v>
+      </c>
+      <c r="F105">
+        <v>1500</v>
+      </c>
+      <c r="G105">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>1500</v>
+      </c>
+      <c r="C106">
+        <v>1500</v>
+      </c>
+      <c r="D106">
+        <v>1500</v>
+      </c>
+      <c r="E106">
+        <v>1500</v>
+      </c>
+      <c r="F106">
+        <v>1500</v>
+      </c>
+      <c r="G106">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>1500</v>
+      </c>
+      <c r="C107">
+        <v>1500</v>
+      </c>
+      <c r="D107">
+        <v>1500</v>
+      </c>
+      <c r="E107">
+        <v>1500</v>
+      </c>
+      <c r="F107">
+        <v>1500</v>
+      </c>
+      <c r="G107">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>1500</v>
+      </c>
+      <c r="C108">
+        <v>1500</v>
+      </c>
+      <c r="D108">
+        <v>1500</v>
+      </c>
+      <c r="E108">
+        <v>1500</v>
+      </c>
+      <c r="F108">
+        <v>1500</v>
+      </c>
+      <c r="G108">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>1500</v>
+      </c>
+      <c r="C109">
+        <v>1500</v>
+      </c>
+      <c r="D109">
+        <v>1500</v>
+      </c>
+      <c r="E109">
+        <v>1500</v>
+      </c>
+      <c r="F109">
+        <v>1500</v>
+      </c>
+      <c r="G109">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>1500</v>
+      </c>
+      <c r="C110">
+        <v>1500</v>
+      </c>
+      <c r="D110">
+        <v>1500</v>
+      </c>
+      <c r="E110">
+        <v>1500</v>
+      </c>
+      <c r="F110">
+        <v>1500</v>
+      </c>
+      <c r="G110">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>1500</v>
+      </c>
+      <c r="C111">
+        <v>1500</v>
+      </c>
+      <c r="D111">
+        <v>1500</v>
+      </c>
+      <c r="E111">
+        <v>1500</v>
+      </c>
+      <c r="F111">
+        <v>1500</v>
+      </c>
+      <c r="G111">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>1500</v>
+      </c>
+      <c r="C112">
+        <v>1500</v>
+      </c>
+      <c r="D112">
+        <v>1500</v>
+      </c>
+      <c r="E112">
+        <v>1500</v>
+      </c>
+      <c r="F112">
+        <v>1500</v>
+      </c>
+      <c r="G112">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>1500</v>
+      </c>
+      <c r="C113">
+        <v>1500</v>
+      </c>
+      <c r="D113">
+        <v>1500</v>
+      </c>
+      <c r="E113">
+        <v>1500</v>
+      </c>
+      <c r="F113">
+        <v>1500</v>
+      </c>
+      <c r="G113">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>1500</v>
+      </c>
+      <c r="C114">
+        <v>1500</v>
+      </c>
+      <c r="D114">
+        <v>1500</v>
+      </c>
+      <c r="E114">
+        <v>1500</v>
+      </c>
+      <c r="F114">
+        <v>1500</v>
+      </c>
+      <c r="G114">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>1500</v>
+      </c>
+      <c r="C115">
+        <v>1500</v>
+      </c>
+      <c r="D115">
+        <v>1500</v>
+      </c>
+      <c r="E115">
+        <v>1500</v>
+      </c>
+      <c r="F115">
+        <v>1500</v>
+      </c>
+      <c r="G115">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>1500</v>
+      </c>
+      <c r="C116">
+        <v>1500</v>
+      </c>
+      <c r="D116">
+        <v>1500</v>
+      </c>
+      <c r="E116">
+        <v>1500</v>
+      </c>
+      <c r="F116">
+        <v>1500</v>
+      </c>
+      <c r="G116">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B117">
+        <v>1500</v>
+      </c>
+      <c r="C117">
+        <v>1500</v>
+      </c>
+      <c r="D117">
+        <v>1500</v>
+      </c>
+      <c r="E117">
+        <v>1500</v>
+      </c>
+      <c r="F117">
+        <v>1500</v>
+      </c>
+      <c r="G117">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>1500</v>
+      </c>
+      <c r="C118">
+        <v>1500</v>
+      </c>
+      <c r="D118">
+        <v>1500</v>
+      </c>
+      <c r="E118">
+        <v>1500</v>
+      </c>
+      <c r="F118">
+        <v>1500</v>
+      </c>
+      <c r="G118">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>1500</v>
+      </c>
+      <c r="C119">
+        <v>1500</v>
+      </c>
+      <c r="D119">
+        <v>1500</v>
+      </c>
+      <c r="E119">
+        <v>1500</v>
+      </c>
+      <c r="F119">
+        <v>1500</v>
+      </c>
+      <c r="G119">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>1500</v>
+      </c>
+      <c r="C120">
+        <v>1500</v>
+      </c>
+      <c r="D120">
+        <v>1500</v>
+      </c>
+      <c r="E120">
+        <v>1500</v>
+      </c>
+      <c r="F120">
+        <v>1500</v>
+      </c>
+      <c r="G120">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>1500</v>
+      </c>
+      <c r="C121">
+        <v>1500</v>
+      </c>
+      <c r="D121">
+        <v>1500</v>
+      </c>
+      <c r="E121">
+        <v>1500</v>
+      </c>
+      <c r="F121">
+        <v>1500</v>
+      </c>
+      <c r="G121">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>1500</v>
+      </c>
+      <c r="C122">
+        <v>1500</v>
+      </c>
+      <c r="D122">
+        <v>1500</v>
+      </c>
+      <c r="E122">
+        <v>1500</v>
+      </c>
+      <c r="F122">
+        <v>1500</v>
+      </c>
+      <c r="G122">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B123">
+        <v>1500</v>
+      </c>
+      <c r="C123">
+        <v>1500</v>
+      </c>
+      <c r="D123">
+        <v>1500</v>
+      </c>
+      <c r="E123">
+        <v>1500</v>
+      </c>
+      <c r="F123">
+        <v>1500</v>
+      </c>
+      <c r="G123">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B124">
+        <v>1500</v>
+      </c>
+      <c r="C124">
+        <v>1500</v>
+      </c>
+      <c r="D124">
+        <v>1500</v>
+      </c>
+      <c r="E124">
+        <v>1500</v>
+      </c>
+      <c r="F124">
+        <v>1500</v>
+      </c>
+      <c r="G124">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B125">
+        <v>1500</v>
+      </c>
+      <c r="C125">
+        <v>1500</v>
+      </c>
+      <c r="D125">
+        <v>1500</v>
+      </c>
+      <c r="E125">
+        <v>1500</v>
+      </c>
+      <c r="F125">
+        <v>1500</v>
+      </c>
+      <c r="G125">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B126">
+        <v>1500</v>
+      </c>
+      <c r="C126">
+        <v>1500</v>
+      </c>
+      <c r="D126">
+        <v>1500</v>
+      </c>
+      <c r="E126">
+        <v>1500</v>
+      </c>
+      <c r="F126">
+        <v>1500</v>
+      </c>
+      <c r="G126">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>1500</v>
+      </c>
+      <c r="C127">
+        <v>1500</v>
+      </c>
+      <c r="D127">
+        <v>1500</v>
+      </c>
+      <c r="E127">
+        <v>1500</v>
+      </c>
+      <c r="F127">
+        <v>1500</v>
+      </c>
+      <c r="G127">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>1500</v>
+      </c>
+      <c r="C128">
+        <v>1500</v>
+      </c>
+      <c r="D128">
+        <v>1500</v>
+      </c>
+      <c r="E128">
+        <v>1500</v>
+      </c>
+      <c r="F128">
+        <v>1500</v>
+      </c>
+      <c r="G128">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>1500</v>
+      </c>
+      <c r="C129">
+        <v>1500</v>
+      </c>
+      <c r="D129">
+        <v>1500</v>
+      </c>
+      <c r="E129">
+        <v>1500</v>
+      </c>
+      <c r="F129">
+        <v>1500</v>
+      </c>
+      <c r="G129">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>1500</v>
+      </c>
+      <c r="C130">
+        <v>1500</v>
+      </c>
+      <c r="D130">
+        <v>1500</v>
+      </c>
+      <c r="E130">
+        <v>1500</v>
+      </c>
+      <c r="F130">
+        <v>1500</v>
+      </c>
+      <c r="G130">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>1500</v>
+      </c>
+      <c r="C131">
+        <v>1500</v>
+      </c>
+      <c r="D131">
+        <v>1500</v>
+      </c>
+      <c r="E131">
+        <v>1500</v>
+      </c>
+      <c r="F131">
+        <v>1500</v>
+      </c>
+      <c r="G131">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>1500</v>
+      </c>
+      <c r="C132">
+        <v>1500</v>
+      </c>
+      <c r="D132">
+        <v>1500</v>
+      </c>
+      <c r="E132">
+        <v>1500</v>
+      </c>
+      <c r="F132">
+        <v>1500</v>
+      </c>
+      <c r="G132">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>1500</v>
+      </c>
+      <c r="C133">
+        <v>1500</v>
+      </c>
+      <c r="D133">
+        <v>1500</v>
+      </c>
+      <c r="E133">
+        <v>1500</v>
+      </c>
+      <c r="F133">
+        <v>1500</v>
+      </c>
+      <c r="G133">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>1500</v>
+      </c>
+      <c r="C134">
+        <v>1500</v>
+      </c>
+      <c r="D134">
+        <v>1500</v>
+      </c>
+      <c r="E134">
+        <v>1500</v>
+      </c>
+      <c r="F134">
+        <v>1500</v>
+      </c>
+      <c r="G134">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>1500</v>
+      </c>
+      <c r="C135">
+        <v>1500</v>
+      </c>
+      <c r="D135">
+        <v>1500</v>
+      </c>
+      <c r="E135">
+        <v>1500</v>
+      </c>
+      <c r="F135">
+        <v>1500</v>
+      </c>
+      <c r="G135">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B136">
+        <v>1500</v>
+      </c>
+      <c r="C136">
+        <v>1500</v>
+      </c>
+      <c r="D136">
+        <v>1500</v>
+      </c>
+      <c r="E136">
+        <v>1500</v>
+      </c>
+      <c r="F136">
+        <v>1500</v>
+      </c>
+      <c r="G136">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B137">
+        <v>1500</v>
+      </c>
+      <c r="C137">
+        <v>1500</v>
+      </c>
+      <c r="D137">
+        <v>1500</v>
+      </c>
+      <c r="E137">
+        <v>1500</v>
+      </c>
+      <c r="F137">
+        <v>1500</v>
+      </c>
+      <c r="G137">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="138" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>1500</v>
+      </c>
+      <c r="C138">
+        <v>1500</v>
+      </c>
+      <c r="D138">
+        <v>1500</v>
+      </c>
+      <c r="E138">
+        <v>1500</v>
+      </c>
+      <c r="F138">
+        <v>1500</v>
+      </c>
+      <c r="G138">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="139" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>1500</v>
+      </c>
+      <c r="C139">
+        <v>1500</v>
+      </c>
+      <c r="D139">
+        <v>1500</v>
+      </c>
+      <c r="E139">
+        <v>1500</v>
+      </c>
+      <c r="F139">
+        <v>1500</v>
+      </c>
+      <c r="G139">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="140" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B140">
+        <v>1500</v>
+      </c>
+      <c r="C140">
+        <v>1500</v>
+      </c>
+      <c r="D140">
+        <v>1500</v>
+      </c>
+      <c r="E140">
+        <v>1500</v>
+      </c>
+      <c r="F140">
+        <v>1500</v>
+      </c>
+      <c r="G140">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="141" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B141">
+        <v>1500</v>
+      </c>
+      <c r="C141">
+        <v>1500</v>
+      </c>
+      <c r="D141">
+        <v>1500</v>
+      </c>
+      <c r="E141">
+        <v>1500</v>
+      </c>
+      <c r="F141">
+        <v>1500</v>
+      </c>
+      <c r="G141">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="142" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B142">
+        <v>1500</v>
+      </c>
+      <c r="C142">
+        <v>1500</v>
+      </c>
+      <c r="D142">
+        <v>1500</v>
+      </c>
+      <c r="E142">
+        <v>1500</v>
+      </c>
+      <c r="F142">
+        <v>1500</v>
+      </c>
+      <c r="G142">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="143" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B143">
+        <v>1500</v>
+      </c>
+      <c r="C143">
+        <v>1500</v>
+      </c>
+      <c r="D143">
+        <v>1500</v>
+      </c>
+      <c r="E143">
+        <v>1500</v>
+      </c>
+      <c r="F143">
+        <v>1500</v>
+      </c>
+      <c r="G143">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="144" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B144">
+        <v>1500</v>
+      </c>
+      <c r="C144">
+        <v>1500</v>
+      </c>
+      <c r="D144">
+        <v>1500</v>
+      </c>
+      <c r="E144">
+        <v>1500</v>
+      </c>
+      <c r="F144">
+        <v>1500</v>
+      </c>
+      <c r="G144">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="145" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B145">
+        <v>1500</v>
+      </c>
+      <c r="C145">
+        <v>1500</v>
+      </c>
+      <c r="D145">
+        <v>1500</v>
+      </c>
+      <c r="E145">
+        <v>1500</v>
+      </c>
+      <c r="F145">
+        <v>1500</v>
+      </c>
+      <c r="G145">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="146" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B146">
+        <v>1500</v>
+      </c>
+      <c r="C146">
+        <v>1500</v>
+      </c>
+      <c r="D146">
+        <v>1500</v>
+      </c>
+      <c r="E146">
+        <v>1500</v>
+      </c>
+      <c r="F146">
+        <v>1500</v>
+      </c>
+      <c r="G146">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="147" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B147">
+        <v>1500</v>
+      </c>
+      <c r="C147">
+        <v>1500</v>
+      </c>
+      <c r="D147">
+        <v>1500</v>
+      </c>
+      <c r="E147">
+        <v>1500</v>
+      </c>
+      <c r="F147">
+        <v>1500</v>
+      </c>
+      <c r="G147">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="148" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B148">
+        <v>1500</v>
+      </c>
+      <c r="C148">
+        <v>1500</v>
+      </c>
+      <c r="D148">
+        <v>1500</v>
+      </c>
+      <c r="E148">
+        <v>1500</v>
+      </c>
+      <c r="F148">
+        <v>1500</v>
+      </c>
+      <c r="G148">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="149" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B149">
+        <v>1500</v>
+      </c>
+      <c r="C149">
+        <v>1500</v>
+      </c>
+      <c r="D149">
+        <v>1500</v>
+      </c>
+      <c r="E149">
+        <v>1500</v>
+      </c>
+      <c r="F149">
+        <v>1500</v>
+      </c>
+      <c r="G149">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="150" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B150">
+        <v>1500</v>
+      </c>
+      <c r="C150">
+        <v>1500</v>
+      </c>
+      <c r="D150">
+        <v>1500</v>
+      </c>
+      <c r="E150">
+        <v>1500</v>
+      </c>
+      <c r="F150">
+        <v>1500</v>
+      </c>
+      <c r="G150">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="151" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B151">
+        <v>1500</v>
+      </c>
+      <c r="C151">
+        <v>1500</v>
+      </c>
+      <c r="D151">
+        <v>1500</v>
+      </c>
+      <c r="E151">
+        <v>1500</v>
+      </c>
+      <c r="F151">
+        <v>1500</v>
+      </c>
+      <c r="G151">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="152" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B152">
+        <v>1500</v>
+      </c>
+      <c r="C152">
+        <v>1500</v>
+      </c>
+      <c r="D152">
+        <v>1500</v>
+      </c>
+      <c r="E152">
+        <v>1500</v>
+      </c>
+      <c r="F152">
+        <v>1500</v>
+      </c>
+      <c r="G152">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="153" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B153">
+        <v>1500</v>
+      </c>
+      <c r="C153">
+        <v>1500</v>
+      </c>
+      <c r="D153">
+        <v>1500</v>
+      </c>
+      <c r="E153">
+        <v>1500</v>
+      </c>
+      <c r="F153">
+        <v>1500</v>
+      </c>
+      <c r="G153">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="154" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B154">
+        <v>1500</v>
+      </c>
+      <c r="C154">
+        <v>1500</v>
+      </c>
+      <c r="D154">
+        <v>1500</v>
+      </c>
+      <c r="E154">
+        <v>1500</v>
+      </c>
+      <c r="F154">
+        <v>1500</v>
+      </c>
+      <c r="G154">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="155" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B155">
+        <v>1500</v>
+      </c>
+      <c r="C155">
+        <v>1500</v>
+      </c>
+      <c r="D155">
+        <v>1500</v>
+      </c>
+      <c r="E155">
+        <v>1500</v>
+      </c>
+      <c r="F155">
+        <v>1500</v>
+      </c>
+      <c r="G155">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="156" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B156">
+        <v>1500</v>
+      </c>
+      <c r="C156">
+        <v>1500</v>
+      </c>
+      <c r="D156">
+        <v>1500</v>
+      </c>
+      <c r="E156">
+        <v>1500</v>
+      </c>
+      <c r="F156">
+        <v>1500</v>
+      </c>
+      <c r="G156">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="157" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B157">
+        <v>1500</v>
+      </c>
+      <c r="C157">
+        <v>1500</v>
+      </c>
+      <c r="D157">
+        <v>1500</v>
+      </c>
+      <c r="E157">
+        <v>1500</v>
+      </c>
+      <c r="F157">
+        <v>1500</v>
+      </c>
+      <c r="G157">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="158" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B158">
+        <v>1500</v>
+      </c>
+      <c r="C158">
+        <v>1500</v>
+      </c>
+      <c r="D158">
+        <v>1500</v>
+      </c>
+      <c r="E158">
+        <v>1500</v>
+      </c>
+      <c r="F158">
+        <v>1500</v>
+      </c>
+      <c r="G158">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="159" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B159">
+        <v>1500</v>
+      </c>
+      <c r="C159">
+        <v>1500</v>
+      </c>
+      <c r="D159">
+        <v>1500</v>
+      </c>
+      <c r="E159">
+        <v>1500</v>
+      </c>
+      <c r="F159">
+        <v>1500</v>
+      </c>
+      <c r="G159">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="160" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B160">
+        <v>1500</v>
+      </c>
+      <c r="C160">
+        <v>1500</v>
+      </c>
+      <c r="D160">
+        <v>1500</v>
+      </c>
+      <c r="E160">
+        <v>1500</v>
+      </c>
+      <c r="F160">
+        <v>1500</v>
+      </c>
+      <c r="G160">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B161">
+        <v>1500</v>
+      </c>
+      <c r="C161">
+        <v>1500</v>
+      </c>
+      <c r="D161">
+        <v>1500</v>
+      </c>
+      <c r="E161">
+        <v>1500</v>
+      </c>
+      <c r="F161">
+        <v>1500</v>
+      </c>
+      <c r="G161">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B162">
+        <v>1500</v>
+      </c>
+      <c r="C162">
+        <v>1500</v>
+      </c>
+      <c r="D162">
+        <v>1500</v>
+      </c>
+      <c r="E162">
+        <v>1500</v>
+      </c>
+      <c r="F162">
+        <v>1500</v>
+      </c>
+      <c r="G162">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B163">
+        <v>1500</v>
+      </c>
+      <c r="C163">
+        <v>1500</v>
+      </c>
+      <c r="D163">
+        <v>1500</v>
+      </c>
+      <c r="E163">
+        <v>1500</v>
+      </c>
+      <c r="F163">
+        <v>1500</v>
+      </c>
+      <c r="G163">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B164">
+        <v>1500</v>
+      </c>
+      <c r="C164">
+        <v>1500</v>
+      </c>
+      <c r="D164">
+        <v>1500</v>
+      </c>
+      <c r="E164">
+        <v>1500</v>
+      </c>
+      <c r="F164">
+        <v>1500</v>
+      </c>
+      <c r="G164">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B165">
+        <v>1500</v>
+      </c>
+      <c r="C165">
+        <v>1500</v>
+      </c>
+      <c r="D165">
+        <v>1500</v>
+      </c>
+      <c r="E165">
+        <v>1500</v>
+      </c>
+      <c r="F165">
+        <v>1500</v>
+      </c>
+      <c r="G165">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B166">
+        <v>1500</v>
+      </c>
+      <c r="C166">
+        <v>1500</v>
+      </c>
+      <c r="D166">
+        <v>1500</v>
+      </c>
+      <c r="E166">
+        <v>1500</v>
+      </c>
+      <c r="F166">
+        <v>1500</v>
+      </c>
+      <c r="G166">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="167" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B167">
+        <v>1500</v>
+      </c>
+      <c r="C167">
+        <v>1500</v>
+      </c>
+      <c r="D167">
+        <v>1500</v>
+      </c>
+      <c r="E167">
+        <v>1500</v>
+      </c>
+      <c r="F167">
+        <v>1500</v>
+      </c>
+      <c r="G167">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B168">
+        <v>1500</v>
+      </c>
+      <c r="C168">
+        <v>1500</v>
+      </c>
+      <c r="D168">
+        <v>1500</v>
+      </c>
+      <c r="E168">
+        <v>1500</v>
+      </c>
+      <c r="F168">
+        <v>1500</v>
+      </c>
+      <c r="G168">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B169">
+        <v>1500</v>
+      </c>
+      <c r="C169">
+        <v>1500</v>
+      </c>
+      <c r="D169">
+        <v>1500</v>
+      </c>
+      <c r="E169">
+        <v>1500</v>
+      </c>
+      <c r="F169">
+        <v>1500</v>
+      </c>
+      <c r="G169">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B170">
+        <v>1500</v>
+      </c>
+      <c r="C170">
+        <v>1500</v>
+      </c>
+      <c r="D170">
+        <v>1500</v>
+      </c>
+      <c r="E170">
+        <v>1500</v>
+      </c>
+      <c r="F170">
+        <v>1500</v>
+      </c>
+      <c r="G170">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="171" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B171">
+        <v>1500</v>
+      </c>
+      <c r="C171">
+        <v>1500</v>
+      </c>
+      <c r="D171">
+        <v>1500</v>
+      </c>
+      <c r="E171">
+        <v>1500</v>
+      </c>
+      <c r="F171">
+        <v>1500</v>
+      </c>
+      <c r="G171">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B172">
+        <v>1500</v>
+      </c>
+      <c r="C172">
+        <v>1500</v>
+      </c>
+      <c r="D172">
+        <v>1500</v>
+      </c>
+      <c r="E172">
+        <v>1500</v>
+      </c>
+      <c r="F172">
+        <v>1500</v>
+      </c>
+      <c r="G172">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B173">
+        <v>1500</v>
+      </c>
+      <c r="C173">
+        <v>1500</v>
+      </c>
+      <c r="D173">
+        <v>1500</v>
+      </c>
+      <c r="E173">
+        <v>1500</v>
+      </c>
+      <c r="F173">
+        <v>1500</v>
+      </c>
+      <c r="G173">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B174">
+        <v>1500</v>
+      </c>
+      <c r="C174">
+        <v>1500</v>
+      </c>
+      <c r="D174">
+        <v>1500</v>
+      </c>
+      <c r="E174">
+        <v>1500</v>
+      </c>
+      <c r="F174">
+        <v>1500</v>
+      </c>
+      <c r="G174">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B175">
+        <v>1500</v>
+      </c>
+      <c r="C175">
+        <v>1500</v>
+      </c>
+      <c r="D175">
+        <v>1500</v>
+      </c>
+      <c r="E175">
+        <v>1500</v>
+      </c>
+      <c r="F175">
+        <v>1500</v>
+      </c>
+      <c r="G175">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="176" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B176">
+        <v>1500</v>
+      </c>
+      <c r="C176">
+        <v>1500</v>
+      </c>
+      <c r="D176">
+        <v>1500</v>
+      </c>
+      <c r="E176">
+        <v>1500</v>
+      </c>
+      <c r="F176">
+        <v>1500</v>
+      </c>
+      <c r="G176">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B177">
+        <v>1500</v>
+      </c>
+      <c r="C177">
+        <v>1500</v>
+      </c>
+      <c r="D177">
+        <v>1500</v>
+      </c>
+      <c r="E177">
+        <v>1500</v>
+      </c>
+      <c r="F177">
+        <v>1500</v>
+      </c>
+      <c r="G177">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="178" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B178">
+        <v>1500</v>
+      </c>
+      <c r="C178">
+        <v>1500</v>
+      </c>
+      <c r="D178">
+        <v>1500</v>
+      </c>
+      <c r="E178">
+        <v>1500</v>
+      </c>
+      <c r="F178">
+        <v>1500</v>
+      </c>
+      <c r="G178">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B179">
+        <v>1500</v>
+      </c>
+      <c r="C179">
+        <v>1500</v>
+      </c>
+      <c r="D179">
+        <v>1500</v>
+      </c>
+      <c r="E179">
+        <v>1500</v>
+      </c>
+      <c r="F179">
+        <v>1500</v>
+      </c>
+      <c r="G179">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B180">
+        <v>1500</v>
+      </c>
+      <c r="C180">
+        <v>1500</v>
+      </c>
+      <c r="D180">
+        <v>1500</v>
+      </c>
+      <c r="E180">
+        <v>1500</v>
+      </c>
+      <c r="F180">
+        <v>1500</v>
+      </c>
+      <c r="G180">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="181" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B181">
+        <v>1500</v>
+      </c>
+      <c r="C181">
+        <v>1500</v>
+      </c>
+      <c r="D181">
+        <v>1500</v>
+      </c>
+      <c r="E181">
+        <v>1500</v>
+      </c>
+      <c r="F181">
+        <v>1500</v>
+      </c>
+      <c r="G181">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="182" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B182">
+        <v>1500</v>
+      </c>
+      <c r="C182">
+        <v>1500</v>
+      </c>
+      <c r="D182">
+        <v>1500</v>
+      </c>
+      <c r="E182">
+        <v>1500</v>
+      </c>
+      <c r="F182">
+        <v>1500</v>
+      </c>
+      <c r="G182">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="183" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B183">
+        <v>1500</v>
+      </c>
+      <c r="C183">
+        <v>1500</v>
+      </c>
+      <c r="D183">
+        <v>1500</v>
+      </c>
+      <c r="E183">
+        <v>1500</v>
+      </c>
+      <c r="F183">
+        <v>1500</v>
+      </c>
+      <c r="G183">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="184" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B184">
+        <v>1500</v>
+      </c>
+      <c r="C184">
+        <v>1500</v>
+      </c>
+      <c r="D184">
+        <v>1500</v>
+      </c>
+      <c r="E184">
+        <v>1500</v>
+      </c>
+      <c r="F184">
+        <v>1500</v>
+      </c>
+      <c r="G184">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="185" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B185">
+        <v>1500</v>
+      </c>
+      <c r="C185">
+        <v>1500</v>
+      </c>
+      <c r="D185">
+        <v>1500</v>
+      </c>
+      <c r="E185">
+        <v>1500</v>
+      </c>
+      <c r="F185">
+        <v>1500</v>
+      </c>
+      <c r="G185">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="186" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B186">
+        <v>1500</v>
+      </c>
+      <c r="C186">
+        <v>1500</v>
+      </c>
+      <c r="D186">
+        <v>1500</v>
+      </c>
+      <c r="E186">
+        <v>1500</v>
+      </c>
+      <c r="F186">
+        <v>1500</v>
+      </c>
+      <c r="G186">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="187" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B187">
+        <v>1500</v>
+      </c>
+      <c r="C187">
+        <v>1500</v>
+      </c>
+      <c r="D187">
+        <v>1500</v>
+      </c>
+      <c r="E187">
+        <v>1500</v>
+      </c>
+      <c r="F187">
+        <v>1500</v>
+      </c>
+      <c r="G187">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="188" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B188">
+        <v>1500</v>
+      </c>
+      <c r="C188">
+        <v>1500</v>
+      </c>
+      <c r="D188">
+        <v>1500</v>
+      </c>
+      <c r="E188">
+        <v>1500</v>
+      </c>
+      <c r="F188">
+        <v>1500</v>
+      </c>
+      <c r="G188">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="189" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B189">
+        <v>1500</v>
+      </c>
+      <c r="C189">
+        <v>1500</v>
+      </c>
+      <c r="D189">
+        <v>1500</v>
+      </c>
+      <c r="E189">
+        <v>1500</v>
+      </c>
+      <c r="F189">
+        <v>1500</v>
+      </c>
+      <c r="G189">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="190" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B190">
+        <v>1500</v>
+      </c>
+      <c r="C190">
+        <v>1500</v>
+      </c>
+      <c r="D190">
+        <v>1500</v>
+      </c>
+      <c r="E190">
+        <v>1500</v>
+      </c>
+      <c r="F190">
+        <v>1500</v>
+      </c>
+      <c r="G190">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="191" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B191">
+        <v>1500</v>
+      </c>
+      <c r="C191">
+        <v>1500</v>
+      </c>
+      <c r="D191">
+        <v>1500</v>
+      </c>
+      <c r="E191">
+        <v>1500</v>
+      </c>
+      <c r="F191">
+        <v>1500</v>
+      </c>
+      <c r="G191">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="192" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B192">
+        <v>1500</v>
+      </c>
+      <c r="C192">
+        <v>1500</v>
+      </c>
+      <c r="D192">
+        <v>1500</v>
+      </c>
+      <c r="E192">
+        <v>1500</v>
+      </c>
+      <c r="F192">
+        <v>1500</v>
+      </c>
+      <c r="G192">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="193" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B193">
+        <v>1500</v>
+      </c>
+      <c r="C193">
+        <v>1500</v>
+      </c>
+      <c r="D193">
+        <v>1500</v>
+      </c>
+      <c r="E193">
+        <v>1500</v>
+      </c>
+      <c r="F193">
+        <v>1500</v>
+      </c>
+      <c r="G193">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="194" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B194">
+        <v>1500</v>
+      </c>
+      <c r="C194">
+        <v>1500</v>
+      </c>
+      <c r="D194">
+        <v>1500</v>
+      </c>
+      <c r="E194">
+        <v>1500</v>
+      </c>
+      <c r="F194">
+        <v>1500</v>
+      </c>
+      <c r="G194">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="195" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B195">
+        <v>1500</v>
+      </c>
+      <c r="C195">
+        <v>1500</v>
+      </c>
+      <c r="D195">
+        <v>1500</v>
+      </c>
+      <c r="E195">
+        <v>1500</v>
+      </c>
+      <c r="F195">
+        <v>1500</v>
+      </c>
+      <c r="G195">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="196" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B196">
+        <v>1500</v>
+      </c>
+      <c r="C196">
+        <v>1500</v>
+      </c>
+      <c r="D196">
+        <v>1500</v>
+      </c>
+      <c r="E196">
+        <v>1500</v>
+      </c>
+      <c r="F196">
+        <v>1500</v>
+      </c>
+      <c r="G196">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="197" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B197">
+        <v>1500</v>
+      </c>
+      <c r="C197">
+        <v>1500</v>
+      </c>
+      <c r="D197">
+        <v>1500</v>
+      </c>
+      <c r="E197">
+        <v>1500</v>
+      </c>
+      <c r="F197">
+        <v>1500</v>
+      </c>
+      <c r="G197">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="198" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B198">
+        <v>1500</v>
+      </c>
+      <c r="C198">
+        <v>1500</v>
+      </c>
+      <c r="D198">
+        <v>1500</v>
+      </c>
+      <c r="E198">
+        <v>1500</v>
+      </c>
+      <c r="F198">
+        <v>1500</v>
+      </c>
+      <c r="G198">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="199" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B199">
+        <v>1500</v>
+      </c>
+      <c r="C199">
+        <v>1500</v>
+      </c>
+      <c r="D199">
+        <v>1500</v>
+      </c>
+      <c r="E199">
+        <v>1500</v>
+      </c>
+      <c r="F199">
+        <v>1500</v>
+      </c>
+      <c r="G199">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="200" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B200">
+        <v>1500</v>
+      </c>
+      <c r="C200">
+        <v>1500</v>
+      </c>
+      <c r="D200">
+        <v>1500</v>
+      </c>
+      <c r="E200">
+        <v>1500</v>
+      </c>
+      <c r="F200">
+        <v>1500</v>
+      </c>
+      <c r="G200">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>